<commit_message>
bivariate analysis and revamp of table one
</commit_message>
<xml_diff>
--- a/internal_datamap_files/DERIVED_covariate_map.xlsx
+++ b/internal_datamap_files/DERIVED_covariate_map.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB3E873-1917-C640-8615-2554C94B161C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD821086-DA13-1243-BA8B-20E6DF8DC6EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="21220" windowHeight="15540" xr2:uid="{32EA9505-1495-5A4A-BC8B-D943AD42845F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="covars" sheetId="1" r:id="rId1"/>
+    <sheet name="old covars" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="160">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -492,9 +493,6 @@
     <t>mapping</t>
   </si>
   <si>
-    <t>risk_factor</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -502,6 +500,12 @@
   </si>
   <si>
     <t>temp_lag_cont_log_scale_clst</t>
+  </si>
+  <si>
+    <t>risk_factor_raw</t>
+  </si>
+  <si>
+    <t>risk_factor_model</t>
   </si>
 </sst>
 </file>
@@ -870,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF2B875-9713-3B46-8F52-EEA3AF9FD86B}">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78:D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -882,7 +886,7 @@
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
@@ -893,10 +897,13 @@
         <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -907,7 +914,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -918,7 +925,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -929,7 +936,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -940,7 +947,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -951,7 +958,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -962,7 +969,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -973,7 +980,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -984,7 +991,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -995,7 +1002,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1006,10 +1013,13 @@
         <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1020,10 +1030,13 @@
         <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1034,7 +1047,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1058,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1056,7 +1069,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1067,10 +1080,13 @@
         <v>115</v>
       </c>
       <c r="D16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1080,8 +1096,11 @@
       <c r="C17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1091,11 +1110,11 @@
       <c r="C18" t="s">
         <v>115</v>
       </c>
-      <c r="D18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1106,10 +1125,13 @@
         <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1119,8 +1141,11 @@
       <c r="C20" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1130,11 +1155,11 @@
       <c r="C21" t="s">
         <v>115</v>
       </c>
-      <c r="D21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1145,10 +1170,13 @@
         <v>115</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1159,10 +1187,13 @@
         <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1172,8 +1203,11 @@
       <c r="C24" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1183,11 +1217,11 @@
       <c r="C25" t="s">
         <v>115</v>
       </c>
-      <c r="D25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1198,10 +1232,13 @@
         <v>115</v>
       </c>
       <c r="D26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1212,10 +1249,13 @@
         <v>115</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1225,8 +1265,11 @@
       <c r="C28" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1236,11 +1279,11 @@
       <c r="C29" t="s">
         <v>115</v>
       </c>
-      <c r="D29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1250,8 +1293,11 @@
       <c r="C30" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1261,11 +1307,11 @@
       <c r="C31" t="s">
         <v>115</v>
       </c>
-      <c r="D31" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>126</v>
       </c>
@@ -1276,10 +1322,13 @@
         <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1290,198 +1339,219 @@
         <v>115</v>
       </c>
       <c r="D33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>141</v>
+      </c>
+      <c r="E40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" t="s">
-        <v>113</v>
-      </c>
-      <c r="C34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C37" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" t="s">
-        <v>119</v>
-      </c>
-      <c r="C38" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" t="s">
-        <v>141</v>
-      </c>
-      <c r="D39" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" t="s">
-        <v>141</v>
-      </c>
-      <c r="D40" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" t="s">
-        <v>141</v>
-      </c>
-      <c r="D41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" t="s">
-        <v>119</v>
-      </c>
-      <c r="C42" t="s">
-        <v>141</v>
-      </c>
-      <c r="D42" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>121</v>
       </c>
-      <c r="C43" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" t="s">
-        <v>120</v>
-      </c>
       <c r="C46" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>157</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
         <v>141</v>
       </c>
-      <c r="D47" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>158</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C48" t="s">
         <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
         <v>122</v>
@@ -1490,9 +1560,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
         <v>122</v>
@@ -1500,38 +1570,47 @@
       <c r="C50" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
         <v>141</v>
       </c>
       <c r="D51" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E51" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C52" t="s">
         <v>141</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
         <v>124</v>
@@ -1540,505 +1619,574 @@
         <v>141</v>
       </c>
       <c r="D53" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>49</v>
-      </c>
-      <c r="B54" t="s">
-        <v>124</v>
+        <v>50</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="C54" t="s">
         <v>141</v>
       </c>
       <c r="D54" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>50</v>
-      </c>
-      <c r="B55" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" t="s">
+        <v>141</v>
+      </c>
+      <c r="D56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" t="s">
+        <v>141</v>
+      </c>
+      <c r="D57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="C58" t="s">
+        <v>141</v>
+      </c>
+      <c r="E58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" t="s">
         <v>128</v>
       </c>
-      <c r="C56" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C59" t="s">
+        <v>141</v>
+      </c>
+      <c r="E59" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" t="s">
         <v>129</v>
       </c>
-      <c r="C57" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C60" t="s">
+        <v>141</v>
+      </c>
+      <c r="E60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" t="s">
         <v>130</v>
       </c>
-      <c r="C58" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>54</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" t="s">
-        <v>141</v>
-      </c>
-      <c r="D59" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" t="s">
-        <v>128</v>
-      </c>
-      <c r="C60" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61" t="s">
-        <v>129</v>
-      </c>
       <c r="C61" t="s">
         <v>141</v>
       </c>
-      <c r="D61" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C62" t="s">
         <v>141</v>
       </c>
       <c r="D62" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" t="s">
+        <v>141</v>
+      </c>
+      <c r="D64" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" t="s">
+        <v>141</v>
+      </c>
+      <c r="D65" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" t="s">
+        <v>141</v>
+      </c>
+      <c r="D66" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" t="s">
+        <v>141</v>
+      </c>
+      <c r="D67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" t="s">
+        <v>141</v>
+      </c>
+      <c r="D68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" t="s">
         <v>131</v>
       </c>
-      <c r="C63" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>59</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C70" t="s">
+        <v>141</v>
+      </c>
+      <c r="E70" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" t="s">
         <v>132</v>
       </c>
-      <c r="C64" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C71" t="s">
+        <v>141</v>
+      </c>
+      <c r="E71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" t="s">
         <v>133</v>
       </c>
-      <c r="C65" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>61</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="C72" t="s">
+        <v>141</v>
+      </c>
+      <c r="E72" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" t="s">
         <v>134</v>
       </c>
-      <c r="C66" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="C73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" t="s">
         <v>135</v>
       </c>
-      <c r="C67" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>63</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="C74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75" t="s">
         <v>136</v>
       </c>
-      <c r="C68" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="C75" t="s">
+        <v>141</v>
+      </c>
+      <c r="E75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76" t="s">
         <v>137</v>
       </c>
-      <c r="C69" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="C76" t="s">
+        <v>141</v>
+      </c>
+      <c r="E76" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>73</v>
+      </c>
+      <c r="B77" t="s">
         <v>138</v>
       </c>
-      <c r="C70" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" t="s">
-        <v>131</v>
-      </c>
-      <c r="C71" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>67</v>
-      </c>
-      <c r="B72" t="s">
-        <v>132</v>
-      </c>
-      <c r="C72" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>68</v>
-      </c>
-      <c r="B73" t="s">
-        <v>133</v>
-      </c>
-      <c r="C73" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>69</v>
-      </c>
-      <c r="B74" t="s">
-        <v>134</v>
-      </c>
-      <c r="C74" t="s">
-        <v>141</v>
-      </c>
-      <c r="D74" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" t="s">
-        <v>135</v>
-      </c>
-      <c r="C75" t="s">
-        <v>141</v>
-      </c>
-      <c r="D75" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>71</v>
-      </c>
-      <c r="B76" t="s">
-        <v>136</v>
-      </c>
-      <c r="C76" t="s">
-        <v>141</v>
-      </c>
-      <c r="D76" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>72</v>
-      </c>
-      <c r="B77" t="s">
-        <v>137</v>
-      </c>
       <c r="C77" t="s">
         <v>141</v>
       </c>
-      <c r="D77" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C78" t="s">
         <v>141</v>
       </c>
       <c r="D78" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B79" t="s">
+        <v>140</v>
+      </c>
+      <c r="C79" t="s">
+        <v>141</v>
+      </c>
+      <c r="D79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>76</v>
+      </c>
+      <c r="B80" t="s">
         <v>139</v>
       </c>
-      <c r="C79" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>75</v>
-      </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" t="s">
         <v>140</v>
       </c>
-      <c r="C80" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>76</v>
-      </c>
-      <c r="B81" t="s">
-        <v>139</v>
-      </c>
       <c r="C81" t="s">
         <v>141</v>
       </c>
-      <c r="D81" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C82" t="s">
-        <v>141</v>
-      </c>
-      <c r="D82" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C83" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C84" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C85" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C86" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C87" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C88" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B89" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C89" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B90" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C90" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B91" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C91" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B92" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C92" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B93" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
       <c r="C93" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B94" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="C94" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>90</v>
-      </c>
-      <c r="B95" t="s">
-        <v>152</v>
-      </c>
-      <c r="C95" t="s">
         <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D7EE9C-5ED9-E344-B332-E49C080F2EB5}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Init Ensemble; Finish Report 1
</commit_message>
<xml_diff>
--- a/internal_datamap_files/DERIVED_covariate_map.xlsx
+++ b/internal_datamap_files/DERIVED_covariate_map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD821086-DA13-1243-BA8B-20E6DF8DC6EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCCB794-300C-5B4D-97C2-09CFAE5CC43B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="21220" windowHeight="15540" xr2:uid="{32EA9505-1495-5A4A-BC8B-D943AD42845F}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="16560" windowHeight="15540" xr2:uid="{32EA9505-1495-5A4A-BC8B-D943AD42845F}"/>
   </bookViews>
   <sheets>
     <sheet name="covars" sheetId="1" r:id="rId1"/>
     <sheet name="old covars" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="167">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -506,13 +506,34 @@
   </si>
   <si>
     <t>risk_factor_model</t>
+  </si>
+  <si>
+    <t>llin_causal_model</t>
+  </si>
+  <si>
+    <t>Distance to Water</t>
+  </si>
+  <si>
+    <t>hlthdist_cont_clst</t>
+  </si>
+  <si>
+    <t>Distance to Healthcare Center</t>
+  </si>
+  <si>
+    <t>wtrdist_cont_log_scale_clst</t>
+  </si>
+  <si>
+    <t>wtrdist_cont_clst</t>
+  </si>
+  <si>
+    <t>hlthdist_cont_log_scale_clst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -531,6 +552,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -556,10 +584,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF2B875-9713-3B46-8F52-EEA3AF9FD86B}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78:D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,7 +915,7 @@
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
@@ -902,8 +931,11 @@
       <c r="E1" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -914,7 +946,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -925,7 +957,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -936,7 +968,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -947,7 +979,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -958,7 +990,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -969,7 +1001,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -980,7 +1012,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -991,7 +1023,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +1034,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1018,8 +1050,9 @@
       <c r="E11" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1035,8 +1068,9 @@
       <c r="E12" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1046,8 +1080,9 @@
       <c r="C13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1058,7 +1093,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1069,7 +1104,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1085,8 +1120,11 @@
       <c r="E16" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1100,7 +1138,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1113,8 +1151,11 @@
       <c r="E18" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1130,8 +1171,11 @@
       <c r="E19" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1145,7 +1189,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1158,8 +1202,11 @@
       <c r="E21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1175,8 +1222,11 @@
       <c r="E22" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1192,8 +1242,11 @@
       <c r="E23" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1207,7 +1260,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1220,8 +1273,11 @@
       <c r="E25" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1237,8 +1293,11 @@
       <c r="E26" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1255,7 +1314,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1269,7 +1328,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1342,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1297,7 +1356,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1310,8 +1369,11 @@
       <c r="E31" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>126</v>
       </c>
@@ -1327,8 +1389,11 @@
       <c r="E32" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1344,8 +1409,11 @@
       <c r="E33" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1359,7 +1427,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1373,7 +1441,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1387,7 +1455,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1401,7 +1469,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1415,7 +1483,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1429,7 +1497,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1443,7 +1511,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1457,7 +1525,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1471,7 +1539,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1485,7 +1553,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1496,7 +1564,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1507,7 +1575,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>156</v>
       </c>
@@ -1520,8 +1588,11 @@
       <c r="E46" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>157</v>
       </c>
@@ -1534,8 +1605,11 @@
       <c r="E47" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -1549,7 +1623,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -1560,7 +1634,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -1573,8 +1647,11 @@
       <c r="E50" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -1591,99 +1668,108 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>165</v>
+      </c>
+      <c r="B52" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" t="s">
+        <v>141</v>
+      </c>
+      <c r="D52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" t="s">
+        <v>155</v>
+      </c>
+      <c r="F53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>48</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>124</v>
       </c>
-      <c r="C52" t="s">
-        <v>141</v>
-      </c>
-      <c r="D52" t="s">
-        <v>155</v>
-      </c>
-      <c r="E52" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="C54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" t="s">
+        <v>155</v>
+      </c>
+      <c r="E54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>49</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>124</v>
       </c>
-      <c r="C53" t="s">
-        <v>141</v>
-      </c>
-      <c r="D53" t="s">
-        <v>155</v>
-      </c>
-      <c r="E53" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="C55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" t="s">
+        <v>155</v>
+      </c>
+      <c r="E55" t="s">
+        <v>155</v>
+      </c>
+      <c r="F55" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" t="s">
+        <v>163</v>
+      </c>
+      <c r="C56" t="s">
+        <v>141</v>
+      </c>
+      <c r="D56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" t="s">
+        <v>163</v>
+      </c>
+      <c r="C57" t="s">
+        <v>141</v>
+      </c>
+      <c r="E57" t="s">
+        <v>155</v>
+      </c>
+      <c r="F57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>50</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" t="s">
-        <v>141</v>
-      </c>
-      <c r="D54" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" t="s">
-        <v>128</v>
-      </c>
-      <c r="C55" t="s">
-        <v>141</v>
-      </c>
-      <c r="D55" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" t="s">
-        <v>129</v>
-      </c>
-      <c r="C56" t="s">
-        <v>141</v>
-      </c>
-      <c r="D56" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" t="s">
-        <v>130</v>
-      </c>
-      <c r="C57" t="s">
-        <v>141</v>
-      </c>
-      <c r="D57" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>54</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>125</v>
@@ -1691,13 +1777,13 @@
       <c r="C58" t="s">
         <v>141</v>
       </c>
-      <c r="E58" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
         <v>128</v>
@@ -1705,13 +1791,13 @@
       <c r="C59" t="s">
         <v>141</v>
       </c>
-      <c r="E59" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B60" t="s">
         <v>129</v>
@@ -1719,13 +1805,13 @@
       <c r="C60" t="s">
         <v>141</v>
       </c>
-      <c r="E60" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
         <v>130</v>
@@ -1733,72 +1819,72 @@
       <c r="C61" t="s">
         <v>141</v>
       </c>
-      <c r="E61" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>58</v>
-      </c>
-      <c r="B62" t="s">
-        <v>131</v>
+        <v>54</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="C62" t="s">
         <v>141</v>
       </c>
-      <c r="D62" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C63" t="s">
         <v>141</v>
       </c>
-      <c r="D63" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C64" t="s">
         <v>141</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
         <v>141</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
         <v>141</v>
@@ -1809,10 +1895,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C67" t="s">
         <v>141</v>
@@ -1823,10 +1909,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
         <v>141</v>
@@ -1837,10 +1923,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C69" t="s">
         <v>141</v>
@@ -1851,66 +1937,66 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C70" t="s">
         <v>141</v>
       </c>
-      <c r="E70" t="s">
+      <c r="D70" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C71" t="s">
         <v>141</v>
       </c>
-      <c r="E71" t="s">
+      <c r="D71" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C72" t="s">
         <v>141</v>
       </c>
-      <c r="E72" t="s">
+      <c r="D72" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B73" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C73" t="s">
         <v>141</v>
       </c>
-      <c r="E73" t="s">
+      <c r="D73" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B74" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C74" t="s">
         <v>141</v>
@@ -1921,10 +2007,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B75" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C75" t="s">
         <v>141</v>
@@ -1935,10 +2021,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B76" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C76" t="s">
         <v>141</v>
@@ -1949,10 +2035,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B77" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C77" t="s">
         <v>141</v>
@@ -1963,200 +2049,268 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B78" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C78" t="s">
         <v>141</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B79" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C79" t="s">
         <v>141</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>73</v>
+      </c>
+      <c r="B81" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" t="s">
+        <v>141</v>
+      </c>
+      <c r="E81" t="s">
+        <v>155</v>
+      </c>
+      <c r="F81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>74</v>
+      </c>
+      <c r="B82" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82" t="s">
+        <v>141</v>
+      </c>
+      <c r="D82" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>75</v>
+      </c>
+      <c r="B83" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" t="s">
+        <v>141</v>
+      </c>
+      <c r="D83" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>76</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B84" t="s">
         <v>139</v>
       </c>
-      <c r="C80" t="s">
-        <v>141</v>
-      </c>
-      <c r="E80" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="C84" t="s">
+        <v>141</v>
+      </c>
+      <c r="E84" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>77</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B85" t="s">
         <v>140</v>
       </c>
-      <c r="C81" t="s">
-        <v>141</v>
-      </c>
-      <c r="E81" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="C85" t="s">
+        <v>141</v>
+      </c>
+      <c r="E85" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>78</v>
       </c>
-      <c r="B82" t="s">
-        <v>141</v>
-      </c>
-      <c r="C82" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" t="s">
-        <v>142</v>
-      </c>
-      <c r="C83" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>80</v>
-      </c>
-      <c r="B84" t="s">
-        <v>143</v>
-      </c>
-      <c r="C84" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>81</v>
-      </c>
-      <c r="B85" t="s">
-        <v>144</v>
-      </c>
-      <c r="C85" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>82</v>
-      </c>
       <c r="B86" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C86" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B87" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C87" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B88" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C88" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B89" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C89" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>82</v>
+      </c>
+      <c r="B90" t="s">
+        <v>145</v>
+      </c>
+      <c r="C90" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>83</v>
+      </c>
+      <c r="B91" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>84</v>
+      </c>
+      <c r="B92" t="s">
+        <v>147</v>
+      </c>
+      <c r="C92" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93" t="s">
+        <v>148</v>
+      </c>
+      <c r="C93" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>86</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B94" t="s">
         <v>149</v>
       </c>
-      <c r="C90" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="C94" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>87</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B95" t="s">
         <v>150</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C95" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="F95" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>88</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B96" t="s">
         <v>151</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C96" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="F96" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>89</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B97" t="s">
         <v>89</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C97" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>90</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B98" t="s">
         <v>152</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C98" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>